<commit_message>
Add document of ThuSoft
</commit_message>
<xml_diff>
--- a/Specifications/Requirement.xlsx
+++ b/Specifications/Requirement.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="14355" windowHeight="5130" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="14355" windowHeight="5130" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Man hinh chinh" sheetId="1" r:id="rId1"/>
     <sheet name="Man hinh input" sheetId="2" r:id="rId2"/>
     <sheet name="Input_nhap ma nhan vien" sheetId="3" r:id="rId3"/>
     <sheet name="Input_nhap hoa don chi tiet" sheetId="4" r:id="rId4"/>
-    <sheet name="Output" sheetId="5" r:id="rId5"/>
-    <sheet name="Output_sắp xếp" sheetId="6" r:id="rId6"/>
-    <sheet name="Output_timkiem" sheetId="7" r:id="rId7"/>
+    <sheet name="Output_timkiem" sheetId="7" r:id="rId5"/>
+    <sheet name="Output" sheetId="5" r:id="rId6"/>
+    <sheet name="Output_sắp xếp" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -553,206 +553,6 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>439360</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76893</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Output.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="685800" y="361950"/>
-          <a:ext cx="8668960" cy="4963218"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>458408</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>134060</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Sapxep.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="723900" y="838200"/>
-          <a:ext cx="8649908" cy="5087060"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>410781</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>38788</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="Sapxep1.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="685800" y="6515100"/>
-          <a:ext cx="8640381" cy="4925113"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>458413</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>162630</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Sapxep2.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="685800" y="11944350"/>
-          <a:ext cx="8688013" cy="5048955"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>496423</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>48339</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="Find.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="685800" y="17735550"/>
-          <a:ext cx="8040223" cy="5115639"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -900,6 +700,206 @@
         <a:xfrm>
           <a:off x="685800" y="15744825"/>
           <a:ext cx="5887272" cy="4505954"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>439360</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76893</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Output.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="361950"/>
+          <a:ext cx="8668960" cy="4963218"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>458408</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>134060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Sapxep.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="838200"/>
+          <a:ext cx="8649908" cy="5087060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>410781</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>38788</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Sapxep1.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="6515100"/>
+          <a:ext cx="8640381" cy="4925113"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>458413</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>162630</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Sapxep2.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="11944350"/>
+          <a:ext cx="8688013" cy="5048955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>496423</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>48339</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Find.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="17735550"/>
+          <a:ext cx="8040223" cy="5115639"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1417,6 +1417,60 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:P93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="L104" sqref="L104"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="12:16">
+      <c r="L35" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+    </row>
+    <row r="85" spans="2:11">
+      <c r="B85" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11">
+      <c r="B86" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11">
+      <c r="K93" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="O4:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1458,7 +1512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:B97"/>
   <sheetViews>
@@ -1487,58 +1541,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="0" copies="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:P93"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="P87" sqref="P87"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="16384" width="9" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:2">
-      <c r="B3" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="12:16">
-      <c r="L35" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-    </row>
-    <row r="85" spans="2:11">
-      <c r="B85" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="86" spans="2:11">
-      <c r="B86" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="93" spans="2:11">
-      <c r="K93" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>